<commit_message>
update parquet data and use sophisticated language and add zoom cercle
</commit_message>
<xml_diff>
--- a/data/data_excel_to_parquet/grappes_regions.xlsx
+++ b/data/data_excel_to_parquet/grappes_regions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\mbarek\script_python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\mbarek\script_python\projet_streamlit\data\data_excel_to_parquet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D07B98-8D6E-49D9-9DF6-5C16F8225226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C25F53-4682-4FC9-A413-678E008BBCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30272E2F-4D00-4F19-8F38-301D085E751F}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,7 +433,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1348</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,7 +441,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1180</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -449,7 +449,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1516</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -457,7 +457,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1023</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -465,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1068</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -473,7 +473,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1086</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -481,7 +481,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1509</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -489,7 +489,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1016</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -497,7 +497,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>